<commit_message>
[add] accuracy 69% val
</commit_message>
<xml_diff>
--- a/temp_submit/COBRE_test_brain_age_submission_소융과_2020105695_김희성_6_15.xlsx
+++ b/temp_submit/COBRE_test_brain_age_submission_소융과_2020105695_김희성_6_15.xlsx
@@ -354,8 +354,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B73"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -376,7 +376,7 @@
         <v>40000</v>
       </c>
       <c r="B2" s="1">
-        <v>41.259131743399699</v>
+        <v>44.078976249067999</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.4">
@@ -384,7 +384,7 @@
         <v>40001</v>
       </c>
       <c r="B3" s="1">
-        <v>49.8489214087042</v>
+        <v>51.092697203883503</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.4">
@@ -392,7 +392,7 @@
         <v>40002</v>
       </c>
       <c r="B4" s="1">
-        <v>51.6126039550523</v>
+        <v>54.373902589237602</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.4">
@@ -400,7 +400,7 @@
         <v>40003</v>
       </c>
       <c r="B5" s="1">
-        <v>44.913513643498</v>
+        <v>48.271624963585801</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.4">
@@ -408,7 +408,7 @@
         <v>40004</v>
       </c>
       <c r="B6" s="1">
-        <v>46.849456037597101</v>
+        <v>46.651265992614398</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.4">
@@ -416,7 +416,7 @@
         <v>40005</v>
       </c>
       <c r="B7" s="1">
-        <v>58.511330867875202</v>
+        <v>63.5080190545874</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.4">
@@ -424,7 +424,7 @@
         <v>40006</v>
       </c>
       <c r="B8" s="1">
-        <v>56.530727527063299</v>
+        <v>52.281367097161201</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.4">
@@ -432,7 +432,7 @@
         <v>40007</v>
       </c>
       <c r="B9" s="1">
-        <v>68.535374156467498</v>
+        <v>65.211545584619401</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.4">
@@ -440,7 +440,7 @@
         <v>40008</v>
       </c>
       <c r="B10" s="1">
-        <v>44.412184829356796</v>
+        <v>49.752055288256798</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.4">
@@ -448,7 +448,7 @@
         <v>40009</v>
       </c>
       <c r="B11" s="1">
-        <v>49.592831415061902</v>
+        <v>51.297537267271501</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.4">
@@ -456,7 +456,7 @@
         <v>40010</v>
       </c>
       <c r="B12" s="1">
-        <v>61.381481500568398</v>
+        <v>60.479717633469001</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.4">
@@ -464,7 +464,7 @@
         <v>40011</v>
       </c>
       <c r="B13" s="1">
-        <v>59.385075099376898</v>
+        <v>56.787098488378902</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.4">
@@ -472,7 +472,7 @@
         <v>40012</v>
       </c>
       <c r="B14" s="1">
-        <v>52.722463430161802</v>
+        <v>58.2017214476692</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.4">
@@ -480,7 +480,7 @@
         <v>40015</v>
       </c>
       <c r="B15" s="1">
-        <v>47.093509983915901</v>
+        <v>50.168146757817198</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.4">
@@ -488,7 +488,7 @@
         <v>40016</v>
       </c>
       <c r="B16" s="1">
-        <v>62.999002917813002</v>
+        <v>65.879618127352202</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.4">
@@ -496,7 +496,7 @@
         <v>40021</v>
       </c>
       <c r="B17" s="1">
-        <v>56.381077505737601</v>
+        <v>57.6138404682115</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.4">
@@ -504,7 +504,7 @@
         <v>40022</v>
       </c>
       <c r="B18" s="1">
-        <v>46.769629352197001</v>
+        <v>55.792555017753102</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.4">
@@ -512,7 +512,7 @@
         <v>40025</v>
       </c>
       <c r="B19" s="1">
-        <v>44.871733146885099</v>
+        <v>49.396279287752101</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.4">
@@ -520,7 +520,7 @@
         <v>40028</v>
       </c>
       <c r="B20" s="1">
-        <v>52.089946533544797</v>
+        <v>62.547170327540897</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.4">
@@ -528,7 +528,7 @@
         <v>40029</v>
       </c>
       <c r="B21" s="1">
-        <v>46.7931160857433</v>
+        <v>54.028989436674998</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.4">
@@ -536,7 +536,7 @@
         <v>40032</v>
       </c>
       <c r="B22" s="1">
-        <v>42.146916969766998</v>
+        <v>45.428433030854997</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.4">
@@ -544,7 +544,7 @@
         <v>40034</v>
       </c>
       <c r="B23" s="1">
-        <v>52.218169277322197</v>
+        <v>54.768350085038598</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.4">
@@ -552,7 +552,7 @@
         <v>40037</v>
       </c>
       <c r="B24" s="1">
-        <v>50.2619974337602</v>
+        <v>48.4073891916075</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.4">
@@ -560,7 +560,7 @@
         <v>40039</v>
       </c>
       <c r="B25" s="1">
-        <v>57.872329460341902</v>
+        <v>56.1644475536933</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.4">
@@ -568,7 +568,7 @@
         <v>40040</v>
       </c>
       <c r="B26" s="1">
-        <v>55.512997718466103</v>
+        <v>58.080732087846997</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.4">
@@ -576,7 +576,7 @@
         <v>40041</v>
       </c>
       <c r="B27" s="1">
-        <v>72.453388431909502</v>
+        <v>67.474923809769905</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.4">
@@ -584,7 +584,7 @@
         <v>40042</v>
       </c>
       <c r="B28" s="1">
-        <v>53.936806013774202</v>
+        <v>55.812893231662301</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.4">
@@ -592,7 +592,7 @@
         <v>40044</v>
       </c>
       <c r="B29" s="1">
-        <v>54.095346152389801</v>
+        <v>52.576520797828501</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.4">
@@ -600,7 +600,7 @@
         <v>40046</v>
       </c>
       <c r="B30" s="1">
-        <v>35.296055313441101</v>
+        <v>52.8140607390662</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.4">
@@ -608,7 +608,7 @@
         <v>40047</v>
       </c>
       <c r="B31" s="1">
-        <v>35.699356182452597</v>
+        <v>40.916123955462403</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.4">
@@ -616,7 +616,7 @@
         <v>40049</v>
       </c>
       <c r="B32" s="1">
-        <v>43.930035082452299</v>
+        <v>51.057367680950897</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.4">
@@ -624,7 +624,7 @@
         <v>40059</v>
       </c>
       <c r="B33" s="1">
-        <v>40.157408707758499</v>
+        <v>44.119733985371099</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.4">
@@ -632,7 +632,7 @@
         <v>40060</v>
       </c>
       <c r="B34" s="1">
-        <v>53.186381189110897</v>
+        <v>56.298681243666202</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.4">
@@ -640,7 +640,7 @@
         <v>40064</v>
       </c>
       <c r="B35" s="1">
-        <v>62.502847379259897</v>
+        <v>60.147762835105198</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.4">
@@ -648,7 +648,7 @@
         <v>40071</v>
       </c>
       <c r="B36" s="1">
-        <v>61.394105924133697</v>
+        <v>62.738564702866903</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.4">
@@ -656,7 +656,7 @@
         <v>40072</v>
       </c>
       <c r="B37" s="1">
-        <v>48.952265645871698</v>
+        <v>57.083664020299999</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.4">
@@ -664,7 +664,7 @@
         <v>40073</v>
       </c>
       <c r="B38" s="1">
-        <v>59.080491428982903</v>
+        <v>61.224693322117197</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.4">
@@ -672,7 +672,7 @@
         <v>40075</v>
       </c>
       <c r="B39" s="1">
-        <v>71.507775219272602</v>
+        <v>68.407517099340694</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.4">
@@ -680,7 +680,7 @@
         <v>40077</v>
       </c>
       <c r="B40" s="1">
-        <v>49.349218744865198</v>
+        <v>55.539008821503202</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.4">
@@ -688,7 +688,7 @@
         <v>40078</v>
       </c>
       <c r="B41" s="1">
-        <v>48.963095979156201</v>
+        <v>50.765420171254</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.4">
@@ -696,7 +696,7 @@
         <v>40079</v>
       </c>
       <c r="B42" s="1">
-        <v>49.695423111820901</v>
+        <v>46.403743894956698</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.4">
@@ -704,7 +704,7 @@
         <v>40080</v>
       </c>
       <c r="B43" s="1">
-        <v>39.814481539139699</v>
+        <v>48.214896516080401</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.4">
@@ -712,7 +712,7 @@
         <v>40081</v>
       </c>
       <c r="B44" s="1">
-        <v>32.842257955502397</v>
+        <v>38.801521577867099</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.4">
@@ -720,7 +720,7 @@
         <v>40082</v>
       </c>
       <c r="B45" s="1">
-        <v>31.550958711799002</v>
+        <v>42.476441402474997</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.4">
@@ -728,7 +728,7 @@
         <v>40084</v>
       </c>
       <c r="B46" s="1">
-        <v>63.5936147693225</v>
+        <v>67.070963512948396</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.4">
@@ -736,7 +736,7 @@
         <v>40085</v>
       </c>
       <c r="B47" s="1">
-        <v>59.477441977206603</v>
+        <v>58.6925956278806</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.4">
@@ -744,7 +744,7 @@
         <v>40088</v>
       </c>
       <c r="B48" s="1">
-        <v>54.916117433916199</v>
+        <v>62.956100730876301</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.4">
@@ -752,7 +752,7 @@
         <v>40089</v>
       </c>
       <c r="B49" s="1">
-        <v>61.246984657172099</v>
+        <v>66.3412933869715</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.4">
@@ -760,7 +760,7 @@
         <v>40092</v>
       </c>
       <c r="B50" s="1">
-        <v>52.849508509583799</v>
+        <v>54.5443455145248</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.4">
@@ -768,7 +768,7 @@
         <v>40094</v>
       </c>
       <c r="B51" s="1">
-        <v>56.354479397172298</v>
+        <v>55.371661756383297</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.4">
@@ -776,7 +776,7 @@
         <v>40096</v>
       </c>
       <c r="B52" s="1">
-        <v>32.8323357095829</v>
+        <v>49.223044252675201</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.4">
@@ -784,7 +784,7 @@
         <v>40097</v>
       </c>
       <c r="B53" s="1">
-        <v>51.713057715349102</v>
+        <v>47.263367371011</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.4">
@@ -792,7 +792,7 @@
         <v>40098</v>
       </c>
       <c r="B54" s="1">
-        <v>55.772963968191597</v>
+        <v>57.438808823446799</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.4">
@@ -800,7 +800,7 @@
         <v>40099</v>
       </c>
       <c r="B55" s="1">
-        <v>37.987499502597601</v>
+        <v>43.489130256925598</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.4">
@@ -808,7 +808,7 @@
         <v>40100</v>
       </c>
       <c r="B56" s="1">
-        <v>59.669886387847399</v>
+        <v>66.188051650142299</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.4">
@@ -816,7 +816,7 @@
         <v>40101</v>
       </c>
       <c r="B57" s="1">
-        <v>62.975774610259798</v>
+        <v>58.435485133667797</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.4">
@@ -824,7 +824,7 @@
         <v>40103</v>
       </c>
       <c r="B58" s="1">
-        <v>37.962529713066999</v>
+        <v>37.161129504195401</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.4">
@@ -832,7 +832,7 @@
         <v>40105</v>
       </c>
       <c r="B59" s="1">
-        <v>66.397481521384194</v>
+        <v>63.6969273197452</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.4">
@@ -840,7 +840,7 @@
         <v>40106</v>
       </c>
       <c r="B60" s="1">
-        <v>57.359079877076297</v>
+        <v>56.257447568449699</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.4">
@@ -848,7 +848,7 @@
         <v>40108</v>
       </c>
       <c r="B61" s="1">
-        <v>60.775804679442899</v>
+        <v>65.1800537091911</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.4">
@@ -856,7 +856,7 @@
         <v>40109</v>
       </c>
       <c r="B62" s="1">
-        <v>47.998312315348699</v>
+        <v>51.984063993124799</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.4">
@@ -864,7 +864,7 @@
         <v>40110</v>
       </c>
       <c r="B63" s="1">
-        <v>40.924245878063999</v>
+        <v>53.489477301848297</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.4">
@@ -872,7 +872,7 @@
         <v>40112</v>
       </c>
       <c r="B64" s="1">
-        <v>51.193926149651503</v>
+        <v>51.748004995355402</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.4">
@@ -880,7 +880,7 @@
         <v>40117</v>
       </c>
       <c r="B65" s="1">
-        <v>49.945933409014202</v>
+        <v>59.527971266005402</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.4">
@@ -888,7 +888,7 @@
         <v>40122</v>
       </c>
       <c r="B66" s="1">
-        <v>51.091704888862203</v>
+        <v>56.129470470847401</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.4">
@@ -896,7 +896,7 @@
         <v>40126</v>
       </c>
       <c r="B67" s="1">
-        <v>54.8133252152452</v>
+        <v>62.957150244474697</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.4">
@@ -904,7 +904,7 @@
         <v>40132</v>
       </c>
       <c r="B68" s="1">
-        <v>45.505045509614398</v>
+        <v>48.432257613953297</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.4">
@@ -912,7 +912,7 @@
         <v>40133</v>
       </c>
       <c r="B69" s="1">
-        <v>49.842035513241903</v>
+        <v>65.182750418630704</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.4">
@@ -920,7 +920,7 @@
         <v>40137</v>
       </c>
       <c r="B70" s="1">
-        <v>45.632219999363002</v>
+        <v>54.582238020310001</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.4">
@@ -928,7 +928,7 @@
         <v>40142</v>
       </c>
       <c r="B71" s="1">
-        <v>47.448054527704898</v>
+        <v>51.1250002212821</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.4">
@@ -936,7 +936,7 @@
         <v>40143</v>
       </c>
       <c r="B72" s="1">
-        <v>60.075069793891899</v>
+        <v>63.261863760880203</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.4">
@@ -944,7 +944,7 @@
         <v>40145</v>
       </c>
       <c r="B73" s="1">
-        <v>31.479177492325</v>
+        <v>46.331298979215198</v>
       </c>
     </row>
   </sheetData>

</xml_diff>